<commit_message>
Implementação parcial do cadastro de de layout das revistas de patente
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
@@ -351,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B3" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -380,6 +380,14 @@
         <v>9.7222222222222224E-2</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>41554</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.20138888888888887</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Início da implementação do cadastro de patente
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
@@ -26,14 +26,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -59,10 +53,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -402,6 +397,14 @@
         <v>0.14583333333333334</v>
       </c>
     </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>41555</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.17361111111111113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Correções e ajustes de acordo com as observações levantadas pelo Hermes
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -405,6 +405,17 @@
         <v>0.17361111111111113</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>41527</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Início de implementação de cadastro de Patentes
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
@@ -355,7 +355,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B7" sqref="B4:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -407,14 +407,19 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>41527</v>
+        <v>41557</v>
       </c>
       <c r="B6" s="3">
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="B7" s="3"/>
+      <c r="A7" s="1">
+        <v>41558</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.1388888888888889</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
Implementação parcial do cadastro de patente
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B4:B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -421,6 +421,22 @@
         <v>0.1388888888888889</v>
       </c>
     </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>41559</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>41560</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.1875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Criação da tela de cadastro de patente
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -437,6 +437,14 @@
         <v>0.1875</v>
       </c>
     </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>41562</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.6805555555555566E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Conclusão da implementação do cadastro de natureza de patente
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B4:B14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -477,6 +477,22 @@
         <v>0.1423611111111111</v>
       </c>
     </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1">
+        <v>41568</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2.4305555555555556E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1">
+        <v>41569</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Início da implementação da funcionalidade de leitura da revista de patente
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B2:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -509,6 +509,46 @@
         <v>7.9861111111111105E-2</v>
       </c>
     </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>41575</v>
+      </c>
+      <c r="B19" s="3">
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>41577</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>41578</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>41580</v>
+      </c>
+      <c r="B22" s="3">
+        <v>6.9444444444444434E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>41581</v>
+      </c>
+      <c r="B23" s="3">
+        <v>9.0277777777777776E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementação parcial da funcionalidade de leitura da revista de patente
</commit_message>
<xml_diff>
--- a/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
+++ b/doc/Projetos/Alternativa Marcas e Patentes LTDA/Apropriações Mauro.xlsx
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B2:B23"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -549,6 +549,14 @@
         <v>9.0277777777777776E-2</v>
       </c>
     </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>41369</v>
+      </c>
+      <c r="B24" s="3">
+        <v>6.25E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>